<commit_message>
update data and add RB model
</commit_message>
<xml_diff>
--- a/results/simple_lstm.xlsx
+++ b/results/simple_lstm.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B119"/>
+  <dimension ref="A1:B83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,1181 +447,821 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>16.54847717285156</v>
+        <v>17.75981712341309</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Ja'Marr Chase</t>
+          <t>Saquon Barkley</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>16.03926658630371</v>
+        <v>14.37493705749512</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Justin Jefferson</t>
+          <t>Derrick Henry</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>14.80686950683594</v>
+        <v>14.05643463134766</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Amon-Ra St. Brown</t>
+          <t>Jahmyr Gibbs</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>12.58254623413086</v>
+        <v>13.79396438598633</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Brian Thomas</t>
+          <t>Bijan Robinson</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>14.71462821960449</v>
+        <v>13.91006278991699</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Terry McLaurin</t>
+          <t>Josh Jacobs</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>13.78668212890625</v>
+        <v>13.2640323638916</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Drake London</t>
+          <t>Kyren Williams</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>15.12775230407715</v>
+        <v>13.11640930175781</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Mike Evans</t>
+          <t>James Cook</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>12.77094173431396</v>
+        <v>14.90402793884277</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Malik Nabers</t>
+          <t>Jonathan Taylor</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>15.40287113189697</v>
+        <v>13.38617706298828</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>CeeDee Lamb</t>
+          <t>De'Von Achane</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>15.90566062927246</v>
+        <v>19.53748321533203</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Courtland Sutton</t>
+          <t>James Conner</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>11.72810363769531</v>
+        <v>20.48888206481934</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Ladd McConkey</t>
+          <t>Joe Mixon</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>17.13962554931641</v>
+        <v>15.67500305175781</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Davante Adams</t>
+          <t>Chase Brown</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>11.63599586486816</v>
+        <v>13.8158540725708</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Jameson Williams</t>
+          <t>Chuba Hubbard</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>11.24908065795898</v>
+        <v>9.244903564453125</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Jaxon Smith-Njigba</t>
+          <t>Bucky Irving</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>14.31130027770996</v>
+        <v>22.51602172851562</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Jerry Jeudy</t>
+          <t>Alvin Kamara</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>13.49443340301514</v>
+        <v>14.79214859008789</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Garrett Wilson</t>
+          <t>Aaron Jones</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>11.23720169067383</v>
+        <v>19.44869804382324</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Jordan Addison</t>
+          <t>David Montgomery</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>13.94121932983398</v>
+        <v>13.63888645172119</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>A.J. Brown</t>
+          <t>Breece Hall</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>16.10597229003906</v>
+        <v>11.62819480895996</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Tee Higgins</t>
+          <t>D'Andre Swift</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>14.90728950500488</v>
+        <v>13.93292808532715</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Nico Collins</t>
+          <t>Najee Harris</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>9.856352806091309</v>
+        <v>17.38212585449219</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Jayden Reed</t>
+          <t>J.K. Dobbins</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>14.91675281524658</v>
+        <v>13.89578819274902</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>D.J. Moore</t>
+          <t>Tony Pollard</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>14.11651992797852</v>
+        <v>9.132762908935547</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Tyreek Hill</t>
+          <t>Rico Dowdle</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>11.46081924438477</v>
+        <v>9.426843643188477</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Zay Flowers</t>
+          <t>Rachaad White</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>9.977712631225586</v>
+        <v>8.231964111328125</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Marvin Harrison Jr.</t>
+          <t>Zach Charbonnet</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>13.20335674285889</v>
+        <v>11.06319236755371</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Calvin Ridley</t>
+          <t>Tyrone Tracy Jr.</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>13.87555503845215</v>
+        <v>13.24843597412109</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Jauan Jennings</t>
+          <t>Rhamondre Stevenson</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>13.60477256774902</v>
+        <v>10.52982330322266</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>DeVonta Smith</t>
+          <t>Brian Robinson Jr.</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>15.54000091552734</v>
+        <v>17.55698013305664</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Jakobi Meyers</t>
+          <t>Kenneth Walker III</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>9.300693511962891</v>
+        <v>9.457186698913574</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Rashod Bateman</t>
+          <t>Kareem Hunt</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>11.67859363555908</v>
+        <v>9.629448890686035</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Darnell Mooney</t>
+          <t>Tank Bigsby</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>14.23297882080078</v>
+        <v>9.754473686218262</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Puka Nacua</t>
+          <t>Javonte Williams</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>9.415665626525879</v>
+        <v>11.4363956451416</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Xavier Worthy</t>
+          <t>Jordan Mason</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>12.47240543365479</v>
+        <v>14.4293212890625</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>D.K. Metcalf</t>
+          <t>Alexander Mattison</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>9.142828941345215</v>
+        <v>6.248634338378906</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Alec Pierce</t>
+          <t>Ray Davis</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>11.38863468170166</v>
+        <v>13.80442905426025</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Quentin Johnston</t>
+          <t>Austin Ekeler</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>15.95917892456055</v>
+        <v>13.35623073577881</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Keenan Allen</t>
+          <t>Jerome Ford</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>10.6760311126709</v>
+        <v>9.713010787963867</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Josh Downs</t>
+          <t>Tyler Allgeier</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>15.5105562210083</v>
+        <v>12.77275657653809</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Cooper Kupp</t>
+          <t>Travis Etienne</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>9.95831298828125</v>
+        <v>10.92727184295654</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Khalil Shakir</t>
+          <t>Jaylen Warren</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>10.46672058105469</v>
+        <v>8.265918731689453</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>George Pickens</t>
+          <t>Ameer Abdullah</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>9.409053802490234</v>
+        <v>8.086188316345215</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Nick Westbrook-Ikhine</t>
+          <t>Justice Hill</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>10.5388126373291</v>
+        <v>8.404445648193359</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Deebo Samuel</t>
+          <t>Emanuel Wilson</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>9.698781967163086</v>
+        <v>9.220335006713867</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Jalen Tolbert</t>
+          <t>Tyjae Spears</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>10.52232360839844</v>
+        <v>9.22382926940918</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Jalen McMillan</t>
+          <t>Antonio Gibson</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>11.3338508605957</v>
+        <v>6.823375701904297</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Michael Pittman Jr.</t>
+          <t>Cam Akers</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>10.00370121002197</v>
+        <v>7.602810382843018</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Demarcus Robinson</t>
+          <t>Isaac Guerendo</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>14.1290111541748</v>
+        <v>8.564052581787109</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Adam Thielen</t>
+          <t>Devin Singletary</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>8.966323852539062</v>
+        <v>6.108110904693604</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Jaylen Waddle</t>
+          <t>Ty Johnson</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>11.16917419433594</v>
+        <v>6.716417789459229</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>DeAndre Hopkins</t>
+          <t>Jaleel McLaughlin</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>7.775283813476562</v>
+        <v>3.549274444580078</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Marvin Mims</t>
+          <t>Braelon Allen</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>8.501726150512695</v>
+        <v>9.768653869628906</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Rome Odunze</t>
+          <t>Gus Edwards</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>9.17530345916748</v>
+        <v>6.22273588180542</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Wan'Dale Robinson</t>
+          <t>Roschon Johnson</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>10.37924480438232</v>
+        <v>6.372236728668213</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Tank Dell</t>
+          <t>Sean Tucker</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>11.69284152984619</v>
+        <v>13.26338768005371</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Allen Lazard</t>
+          <t>Zack Moss</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>16.79556083679199</v>
+        <v>12.04964637756348</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Chris Godwin</t>
+          <t>Nick Chubb</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>10.66602611541748</v>
+        <v>7.571753978729248</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Romeo Doubs</t>
+          <t>Jeremy McNichols</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>7.969696044921875</v>
+        <v>7.486612796783447</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Andrei Iosivas</t>
+          <t>Samaje Perine</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>7.009440422058105</v>
+        <v>9.37612247467041</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Calvin Austin III</t>
+          <t>Miles Sanders</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>9.128079414367676</v>
+        <v>11.00978183746338</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Keon Coleman</t>
+          <t>Raheem Mostert</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>7.717312812805176</v>
+        <v>7.466166019439697</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Demario Douglas</t>
+          <t>Kenneth Gainwell</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>9.394969940185547</v>
+        <v>7.829729557037354</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Tre Tucker</t>
+          <t>Ezekiel Elliott</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>8.932703018188477</v>
+        <v>11.78047752380371</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Kayshon Boutte</t>
+          <t>Isiah Pacheco</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>12.39778327941895</v>
+        <v>7.110752582550049</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Amari Cooper</t>
+          <t>Audric Estime</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>7.716930389404297</v>
+        <v>8.583818435668945</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Ray-Ray McCloud</t>
+          <t>Dameon Pierce</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>8.544332504272461</v>
+        <v>6.860898971557617</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Michael Wilson</t>
+          <t>Trey Benson</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>9.729764938354492</v>
+        <v>7.789467334747314</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Xavier Legette</t>
+          <t>Emari Demercado</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>6.58043384552002</v>
+        <v>6.351815700531006</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Christian Watson</t>
+          <t>Trey Sermon</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>16.63986587524414</v>
+        <v>5.528404235839844</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Stefon Diggs</t>
+          <t>Isaiah Davis</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>6.635261535644531</v>
+        <v>8.090071678161621</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Jalen Nailor</t>
+          <t>Dare Ogunbowale</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>8.149435997009277</v>
+        <v>6.022610664367676</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>KaVontae Turpin</t>
+          <t>Tyler Goodson</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>9.145547866821289</v>
+        <v>17.86209869384766</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Tyler Lockett</t>
+          <t>Christian McCaffrey</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>9.297714233398438</v>
+        <v>6.679512500762939</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Dontayvion Wicks</t>
+          <t>Chris Brooks</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>8.03706169128418</v>
+        <v>7.61220121383667</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Darius Slayton</t>
+          <t>Chris Rodriguez</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>8.796413421630859</v>
+        <v>5.529768466949463</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Mack Hollins</t>
+          <t>Hassan Haskins</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>7.342109680175781</v>
+        <v>6.474011898040771</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Josh Palmer</t>
+          <t>Kimani Vidal</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>6.984540939331055</v>
+        <v>7.44008207321167</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Olamide Zaccheaus</t>
+          <t>Jamaal Williams</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>9.169837951660156</v>
+        <v>6.44995641708374</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Marquez Valdes-Scantling</t>
+          <t>Blake Corum</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>8.384590148925781</v>
+        <v>8.184813499450684</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Devaughn Vele</t>
+          <t>D'Onta Foreman</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>7.045717239379883</v>
+        <v>7.448765754699707</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Parker Washington</t>
+          <t>Patrick Taylor</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>8.366110801696777</v>
+        <v>8.509670257568359</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Ricky Pearsall</t>
+          <t>Cordarrelle Patterson</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>7.916900634765625</v>
+        <v>14.40653133392334</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Jalen Coker</t>
-        </is>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="n">
-        <v>8.091597557067871</v>
-      </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>Elijah Moore</t>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="n">
-        <v>12.23458480834961</v>
-      </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>Rashid Shaheed</t>
-        </is>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="n">
-        <v>7.695537567138672</v>
-      </c>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>Tim Patrick</t>
-        </is>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="n">
-        <v>5.678319931030273</v>
-      </c>
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>Tutu Atwell</t>
-        </is>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="n">
-        <v>11.09529876708984</v>
-      </c>
-      <c r="B88" t="inlineStr">
-        <is>
-          <t>Diontae Johnson</t>
-        </is>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="n">
-        <v>6.613827705383301</v>
-      </c>
-      <c r="B89" t="inlineStr">
-        <is>
-          <t>Greg Dortch</t>
-        </is>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="n">
-        <v>8.442317008972168</v>
-      </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>David Moore</t>
-        </is>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="n">
-        <v>9.387294769287109</v>
-      </c>
-      <c r="B91" t="inlineStr">
-        <is>
-          <t>Noah Brown</t>
-        </is>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="n">
-        <v>8.262104988098145</v>
-      </c>
-      <c r="B92" t="inlineStr">
-        <is>
-          <t>Cedric Tillman</t>
-        </is>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="n">
-        <v>9.207879066467285</v>
-      </c>
-      <c r="B93" t="inlineStr">
-        <is>
-          <t>Sterling Shepard</t>
-        </is>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="n">
-        <v>8.863238334655762</v>
-      </c>
-      <c r="B94" t="inlineStr">
-        <is>
-          <t>Chris Olave</t>
-        </is>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="n">
-        <v>12.16502952575684</v>
-      </c>
-      <c r="B95" t="inlineStr">
-        <is>
-          <t>Brandin Cooks</t>
-        </is>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="n">
-        <v>10.92100715637207</v>
-      </c>
-      <c r="B96" t="inlineStr">
-        <is>
-          <t>Christian Kirk</t>
-        </is>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="n">
-        <v>11.90900230407715</v>
-      </c>
-      <c r="B97" t="inlineStr">
-        <is>
-          <t>Rashee Rice</t>
-        </is>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="n">
-        <v>6.64690113067627</v>
-      </c>
-      <c r="B98" t="inlineStr">
-        <is>
-          <t>Justin Watson</t>
-        </is>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="n">
-        <v>7.218036651611328</v>
-      </c>
-      <c r="B99" t="inlineStr">
-        <is>
-          <t>Van Jefferson</t>
-        </is>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="n">
-        <v>8.259385108947754</v>
-      </c>
-      <c r="B100" t="inlineStr">
-        <is>
-          <t>Kalif Raymond</t>
-        </is>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="n">
-        <v>7.3756103515625</v>
-      </c>
-      <c r="B101" t="inlineStr">
-        <is>
-          <t>Tyler Boyd</t>
-        </is>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" t="n">
-        <v>6.921442031860352</v>
-      </c>
-      <c r="B102" t="inlineStr">
-        <is>
-          <t>Troy Franklin</t>
-        </is>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" t="n">
-        <v>10.07075023651123</v>
-      </c>
-      <c r="B103" t="inlineStr">
-        <is>
-          <t>Brandon Aiyuk</t>
-        </is>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" t="n">
-        <v>8.036118507385254</v>
-      </c>
-      <c r="B104" t="inlineStr">
-        <is>
-          <t>Kendrick Bourne</t>
-        </is>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" t="n">
-        <v>5.647940635681152</v>
-      </c>
-      <c r="B105" t="inlineStr">
-        <is>
-          <t>Dyami Brown</t>
-        </is>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="n">
-        <v>6.562331199645996</v>
-      </c>
-      <c r="B106" t="inlineStr">
-        <is>
-          <t>Mike Williams</t>
-        </is>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" t="n">
-        <v>7.981444358825684</v>
-      </c>
-      <c r="B107" t="inlineStr">
-        <is>
-          <t>Nelson Agholor</t>
-        </is>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" t="n">
-        <v>6.575793266296387</v>
-      </c>
-      <c r="B108" t="inlineStr">
-        <is>
-          <t>Tyler Johnson</t>
-        </is>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" t="n">
-        <v>7.271862983703613</v>
-      </c>
-      <c r="B109" t="inlineStr">
-        <is>
-          <t>JuJu Smith-Schuster</t>
-        </is>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" t="n">
-        <v>8.050222396850586</v>
-      </c>
-      <c r="B110" t="inlineStr">
-        <is>
-          <t>Gabriel Davis</t>
-        </is>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" t="n">
-        <v>6.015207290649414</v>
-      </c>
-      <c r="B111" t="inlineStr">
-        <is>
-          <t>Lil'Jordan Humphrey</t>
-        </is>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" t="n">
-        <v>7.812981605529785</v>
-      </c>
-      <c r="B112" t="inlineStr">
-        <is>
-          <t>Curtis Samuel</t>
-        </is>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" t="n">
-        <v>6.073528289794922</v>
-      </c>
-      <c r="B113" t="inlineStr">
-        <is>
-          <t>John Metchie</t>
-        </is>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" t="n">
-        <v>6.347736358642578</v>
-      </c>
-      <c r="B114" t="inlineStr">
-        <is>
-          <t>Adonai Mitchell</t>
-        </is>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" t="n">
-        <v>8.018453598022461</v>
-      </c>
-      <c r="B115" t="inlineStr">
-        <is>
-          <t>DJ Turner</t>
-        </is>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" t="n">
-        <v>4.933768272399902</v>
-      </c>
-      <c r="B116" t="inlineStr">
-        <is>
-          <t>Jordan Whittington</t>
-        </is>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117" t="n">
-        <v>7.055644989013672</v>
-      </c>
-      <c r="B117" t="inlineStr">
-        <is>
-          <t>Cedrick Wilson Jr.</t>
-        </is>
-      </c>
-    </row>
-    <row r="118">
-      <c r="A118" t="n">
-        <v>5.482773780822754</v>
-      </c>
-      <c r="B118" t="inlineStr">
-        <is>
-          <t>Malik Washington</t>
-        </is>
-      </c>
-    </row>
-    <row r="119">
-      <c r="A119" t="n">
-        <v>5.606703758239746</v>
-      </c>
-      <c r="B119" t="inlineStr">
-        <is>
-          <t>Derius Davis</t>
+          <t>Michael Carter</t>
         </is>
       </c>
     </row>

</xml_diff>